<commit_message>
#16 Entering medication values
+ some small changes
</commit_message>
<xml_diff>
--- a/adapter/report-generator/excel-report-generator/src/main/resources/report_template.xlsx
+++ b/adapter/report-generator/excel-report-generator/src/main/resources/report_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domenic\Dropbox\Studium\Semester\7. Semester\Arbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domenic\IdeaProjects\HearthCapture\adapter\report-generator\excel-report-generator\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E3807B-C9BE-405E-9196-AAD395409312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5E0078-F5FF-469A-B918-E4666E5672FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-195" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="198">
   <si>
     <t>Datum</t>
   </si>
@@ -218,9 +218,6 @@
     <t>Plättchenaggregationshemmer</t>
   </si>
   <si>
-    <t>Arterenol</t>
-  </si>
-  <si>
     <t>Vasopressin</t>
   </si>
   <si>
@@ -296,9 +293,6 @@
     <t>SOFA Score</t>
   </si>
   <si>
-    <t>Nitro</t>
-  </si>
-  <si>
     <t>Antibiotika</t>
   </si>
   <si>
@@ -407,9 +401,6 @@
     <t>Impella präoperativ</t>
   </si>
   <si>
-    <t>Dosis</t>
-  </si>
-  <si>
     <t>0/1</t>
   </si>
   <si>
@@ -422,9 +413,6 @@
     <t>Medikamente präoperativ</t>
   </si>
   <si>
-    <t>iv Medikamente präoperativ</t>
-  </si>
-  <si>
     <t>Labor präoperativ</t>
   </si>
   <si>
@@ -732,6 +720,21 @@
   </si>
   <si>
     <t>LACTAT_ven</t>
+  </si>
+  <si>
+    <t>Laufrate</t>
+  </si>
+  <si>
+    <t>Medikamente prä-HLM</t>
+  </si>
+  <si>
+    <t>Norepinephrin</t>
+  </si>
+  <si>
+    <t>Milrinon</t>
+  </si>
+  <si>
+    <t>NTG</t>
   </si>
 </sst>
 </file>
@@ -1574,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="BA164" sqref="BA164"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,7 +1631,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1641,12 +1644,12 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="e">
         <f>B8/(B7/100*B7/100)</f>
@@ -1655,74 +1658,74 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1">
-        <f>((B7*B8)/3600)^1/2</f>
+        <f>D10</f>
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>2.6</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1">
         <f>B10*B11</f>
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1730,7 +1733,7 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1738,12 +1741,12 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1751,17 +1754,17 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1776,43 +1779,43 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1820,77 +1823,82 @@
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
         <v>86</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1898,176 +1906,214 @@
         <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>194</v>
+      </c>
+      <c r="B95" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2083,12 +2129,12 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -2099,7 +2145,7 @@
         <v>0</v>
       </c>
       <c r="C110" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2110,15 +2156,15 @@
         <v>0</v>
       </c>
       <c r="C111" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B112" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2126,39 +2172,39 @@
         <v>14</v>
       </c>
       <c r="B113" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B114" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B115" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B116" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B117" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2173,81 +2219,81 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C138" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C141" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C143" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="164" spans="1:83" x14ac:dyDescent="0.25">
@@ -2255,34 +2301,34 @@
         <v>15</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I164" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J164" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K164" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L164" s="3" t="s">
         <v>16</v>
@@ -2291,211 +2337,211 @@
         <v>21</v>
       </c>
       <c r="N164" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="O164" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="P164" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q164" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="R164" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="S164" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T164" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="U164" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="V164" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="W164" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="X164" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y164" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z164" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA164" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB164" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC164" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD164" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE164" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF164" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG164" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH164" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI164" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ164" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK164" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL164" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM164" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN164" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AO164" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP164" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AQ164" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AR164" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AS164" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AT164" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="O164" s="5" t="s">
+      <c r="AU164" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AV164" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW164" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="AX164" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AY164" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AZ164" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="BA164" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="BB164" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="BC164" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="P164" s="5" t="s">
+      <c r="BD164" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="Q164" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="R164" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="S164" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T164" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="U164" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="V164" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="W164" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="X164" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y164" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z164" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA164" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB164" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC164" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD164" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE164" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="AF164" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="AG164" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="AH164" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI164" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ164" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="AK164" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="AL164" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="AM164" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN164" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="AO164" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP164" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="AQ164" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="AR164" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="AS164" s="3" t="s">
+      <c r="BE164" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="AT164" s="3" t="s">
+      <c r="BF164" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="AU164" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AV164" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="AW164" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="AX164" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="AY164" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="AZ164" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="BA164" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="BB164" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="BC164" s="3" t="s">
+      <c r="BG164" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="BD164" s="3" t="s">
+      <c r="BH164" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="BE164" s="3" t="s">
+      <c r="BI164" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="BF164" s="3" t="s">
+      <c r="BJ164" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="BG164" s="3" t="s">
+      <c r="BK164" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="BH164" s="3" t="s">
+      <c r="BL164" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="BI164" s="3" t="s">
+      <c r="BM164" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="BJ164" s="3" t="s">
+      <c r="BN164" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="BK164" s="3" t="s">
+      <c r="BO164" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="BL164" s="3" t="s">
+      <c r="BP164" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="BM164" s="3" t="s">
+      <c r="BQ164" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="BN164" s="3" t="s">
+      <c r="BR164" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="BO164" s="3" t="s">
+      <c r="BS164" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="BP164" s="3" t="s">
+      <c r="BT164" t="s">
         <v>182</v>
       </c>
-      <c r="BQ164" s="3" t="s">
+      <c r="BU164" t="s">
         <v>183</v>
       </c>
-      <c r="BR164" s="3" t="s">
+      <c r="BV164" t="s">
         <v>184</v>
       </c>
-      <c r="BS164" s="3" t="s">
+      <c r="BW164" t="s">
         <v>185</v>
       </c>
-      <c r="BT164" t="s">
+      <c r="BX164" t="s">
         <v>186</v>
       </c>
-      <c r="BU164" t="s">
+      <c r="BY164" t="s">
         <v>187</v>
       </c>
-      <c r="BV164" t="s">
+      <c r="BZ164" t="s">
         <v>188</v>
       </c>
-      <c r="BW164" t="s">
+      <c r="CA164" t="s">
         <v>189</v>
       </c>
-      <c r="BX164" t="s">
+      <c r="CB164" t="s">
         <v>190</v>
       </c>
-      <c r="BY164" t="s">
+      <c r="CC164" t="s">
         <v>191</v>
       </c>
-      <c r="BZ164" t="s">
+      <c r="CD164" t="s">
         <v>192</v>
-      </c>
-      <c r="CA164" t="s">
-        <v>193</v>
-      </c>
-      <c r="CB164" t="s">
-        <v>194</v>
-      </c>
-      <c r="CC164" t="s">
-        <v>195</v>
-      </c>
-      <c r="CD164" t="s">
-        <v>196</v>
       </c>
       <c r="CE164" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Hotfix for KOF in template file
</commit_message>
<xml_diff>
--- a/adapter/report-generator/excel-report-generator/src/main/resources/report_template.xlsx
+++ b/adapter/report-generator/excel-report-generator/src/main/resources/report_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domenic\IdeaProjects\HearthCapture\adapter\report-generator\excel-report-generator\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5E0078-F5FF-469A-B918-E4666E5672FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FF6F29-EED4-4752-9CCA-23B7E1FDCF7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,7 +1661,7 @@
         <v>39</v>
       </c>
       <c r="B10" s="1">
-        <f>D10</f>
+        <f>((B7*B8)/3600)^1/2</f>
         <v>0</v>
       </c>
       <c r="C10" t="s">

</xml_diff>